<commit_message>
20251022 Folder monitor update
</commit_message>
<xml_diff>
--- a/GUI + Reviews - Copy/202506/Developed Market.xlsx
+++ b/GUI + Reviews - Copy/202506/Developed Market.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://euronext-my.sharepoint.com/personal/csonneveld_euronext_com/Documents/Documents/Projects/GUI + Reviews/202506/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C219A4C4-4086-4094-9BA9-B15529C1D2F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{C219A4C4-4086-4094-9BA9-B15529C1D2F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{054E7AB8-8F54-451A-A881-F0B6FC4B9A90}"/>
   <bookViews>
-    <workbookView xWindow="-27225" yWindow="-11955" windowWidth="27195" windowHeight="12930" xr2:uid="{5B94506A-FB95-4D77-92CD-2774C1C6A4EA}"/>
+    <workbookView xWindow="-24825" yWindow="2580" windowWidth="21600" windowHeight="11295" xr2:uid="{5B94506A-FB95-4D77-92CD-2774C1C6A4EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14669,8 +14669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36D0DE39-3A49-4FD8-8121-C8D2F22CB5BD}">
   <dimension ref="A1:K1542"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" topLeftCell="A994" workbookViewId="0">
+      <selection activeCell="M1000" sqref="M1000"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15895,10 +15895,10 @@
         <v>87</v>
       </c>
       <c r="F35" s="1">
-        <v>150000000</v>
+        <v>1500000000</v>
       </c>
       <c r="G35" s="1">
-        <v>238.2</v>
+        <v>23.82</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>38</v>
@@ -17820,7 +17820,7 @@
         <v>14</v>
       </c>
       <c r="F90" s="1">
-        <v>1337577900</v>
+        <v>1178050260</v>
       </c>
       <c r="G90" s="1">
         <v>26.072179999999999</v>
@@ -37805,10 +37805,10 @@
         <v>114</v>
       </c>
       <c r="F661" s="1">
-        <v>108958830</v>
+        <v>435835320</v>
       </c>
       <c r="G661" s="1">
-        <v>182.12350000000001</v>
+        <v>45.530875000000002</v>
       </c>
       <c r="H661" s="1" t="s">
         <v>21</v>
@@ -38645,7 +38645,7 @@
         <v>37</v>
       </c>
       <c r="F685" s="1">
-        <v>811753913</v>
+        <v>1014692391</v>
       </c>
       <c r="G685" s="1">
         <v>7.15</v>
@@ -49915,10 +49915,10 @@
         <v>114</v>
       </c>
       <c r="F1007" s="1">
-        <v>56989456</v>
+        <v>854841840</v>
       </c>
       <c r="G1007" s="1">
-        <v>1211.4860000000001</v>
+        <v>80.765733330000003</v>
       </c>
       <c r="H1007" s="1" t="s">
         <v>21</v>

</xml_diff>